<commit_message>
Add Hydro plants from https://github.com/energy-modelling-toolkit/hydro-power-database Recalculate NTCs from commercial exchnage. Merge CTA/CTY Values for borders where only one is available (e.g. IT-CH)
</commit_message>
<xml_diff>
--- a/data_in/data_structure.xlsx
+++ b/data_in/data_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riw\Documents\repositories\pomato_data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78B4AEB-EFCE-429A-8ECC-6AD2F13FC469}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150F1EDD-E23A-456B-81A7-010C77E7A826}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="0" windowWidth="16800" windowHeight="17280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-108" windowWidth="40548" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="101">
   <si>
     <t xml:space="preserve">Attribute </t>
   </si>
@@ -320,6 +320,15 @@
   </si>
   <si>
     <t>plants.index</t>
+  </si>
+  <si>
+    <t>d_max</t>
+  </si>
+  <si>
+    <t>inflows</t>
+  </si>
+  <si>
+    <t>inflow</t>
   </si>
 </sst>
 </file>
@@ -1080,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AF25"/>
+  <dimension ref="A1:AF26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1183,10 +1192,10 @@
       <c r="AD1" t="s">
         <v>65</v>
       </c>
-      <c r="AE1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AE1" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF1" s="14" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1281,11 +1290,11 @@
       <c r="AD2" t="s">
         <v>65</v>
       </c>
-      <c r="AE2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>65</v>
+      <c r="AE2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
@@ -1380,10 +1389,10 @@
         <v>65</v>
       </c>
       <c r="AE3" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="AF3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
@@ -1478,10 +1487,10 @@
         <v>65</v>
       </c>
       <c r="AE4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="AF4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
@@ -1576,10 +1585,10 @@
         <v>65</v>
       </c>
       <c r="AE5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AF5" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
@@ -1674,10 +1683,10 @@
         <v>65</v>
       </c>
       <c r="AE6" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="AF6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
@@ -1759,12 +1768,6 @@
       <c r="AD7" t="s">
         <v>65</v>
       </c>
-      <c r="AE7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="8" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1851,10 +1854,10 @@
       <c r="AD8" t="s">
         <v>65</v>
       </c>
-      <c r="AE8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF8" t="s">
+      <c r="AE8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF8" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3386,8 +3389,17 @@
         <v>69</v>
       </c>
     </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>

</xml_diff>

<commit_message>
Trying out riws 29-05 data_out
</commit_message>
<xml_diff>
--- a/data_in/data_structure.xlsx
+++ b/data_in/data_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riw\Documents\repositories\pomato_data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78B4AEB-EFCE-429A-8ECC-6AD2F13FC469}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150F1EDD-E23A-456B-81A7-010C77E7A826}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="0" windowWidth="16800" windowHeight="17280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-108" windowWidth="40548" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="101">
   <si>
     <t xml:space="preserve">Attribute </t>
   </si>
@@ -320,6 +320,15 @@
   </si>
   <si>
     <t>plants.index</t>
+  </si>
+  <si>
+    <t>d_max</t>
+  </si>
+  <si>
+    <t>inflows</t>
+  </si>
+  <si>
+    <t>inflow</t>
   </si>
 </sst>
 </file>
@@ -1080,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AF25"/>
+  <dimension ref="A1:AF26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1183,10 +1192,10 @@
       <c r="AD1" t="s">
         <v>65</v>
       </c>
-      <c r="AE1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AE1" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF1" s="14" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1281,11 +1290,11 @@
       <c r="AD2" t="s">
         <v>65</v>
       </c>
-      <c r="AE2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>65</v>
+      <c r="AE2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
@@ -1380,10 +1389,10 @@
         <v>65</v>
       </c>
       <c r="AE3" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="AF3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
@@ -1478,10 +1487,10 @@
         <v>65</v>
       </c>
       <c r="AE4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="AF4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
@@ -1576,10 +1585,10 @@
         <v>65</v>
       </c>
       <c r="AE5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="AF5" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
@@ -1674,10 +1683,10 @@
         <v>65</v>
       </c>
       <c r="AE6" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="AF6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
@@ -1759,12 +1768,6 @@
       <c r="AD7" t="s">
         <v>65</v>
       </c>
-      <c r="AE7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="8" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1851,10 +1854,10 @@
       <c r="AD8" t="s">
         <v>65</v>
       </c>
-      <c r="AE8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF8" t="s">
+      <c r="AE8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF8" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3386,8 +3389,17 @@
         <v>69</v>
       </c>
     </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>

</xml_diff>

<commit_message>
Include entso-e weekly storage level for hydro reservoirs. Minor cleanup update readme
</commit_message>
<xml_diff>
--- a/data_in/data_structure.xlsx
+++ b/data_in/data_structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riw\Documents\repositories\pomato_data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150F1EDD-E23A-456B-81A7-010C77E7A826}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59BD49F-B238-4106-B41D-1414D5C50399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="40548" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="102">
   <si>
     <t xml:space="preserve">Attribute </t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>inflow</t>
+  </si>
+  <si>
+    <t>storage_level</t>
   </si>
 </sst>
 </file>
@@ -1089,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AF26"/>
+  <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB14" sqref="AB14"/>
+      <selection activeCell="AH16" sqref="AH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,7 +1108,7 @@
     <col min="28" max="28" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -1198,8 +1201,14 @@
       <c r="AF1" s="14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AH1" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI1" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
@@ -1296,8 +1305,14 @@
       <c r="AF2" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AH2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1394,8 +1409,14 @@
       <c r="AF3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AH3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1492,8 +1513,14 @@
       <c r="AF4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AH4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1590,8 +1617,14 @@
       <c r="AF5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AH5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1688,8 +1721,14 @@
       <c r="AF6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AH6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1769,7 +1808,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1860,8 +1899,14 @@
       <c r="AF8" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AH8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI8" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>87</v>
       </c>
@@ -1959,7 +2004,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2057,7 +2102,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2149,7 +2194,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -2241,7 +2286,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -2339,7 +2384,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -2437,7 +2482,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -2529,7 +2574,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -3398,7 +3443,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Update: DE OPSD 2020 smaller fixes and changes
</commit_message>
<xml_diff>
--- a/data_in/data_structure.xlsx
+++ b/data_in/data_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riw\Documents\repositories\pomato_data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59BD49F-B238-4106-B41D-1414D5C50399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7629170-6264-4D14-B340-AD8DD7DDEAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-108" windowWidth="40548" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="0" windowWidth="23520" windowHeight="17280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="104">
   <si>
     <t xml:space="preserve">Attribute </t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>storage_level</t>
+  </si>
+  <si>
+    <t>heatareas</t>
+  </si>
+  <si>
+    <t>demand_h</t>
   </si>
 </sst>
 </file>
@@ -1092,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AI26"/>
+  <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH16" sqref="AH16"/>
+    <sheetView tabSelected="1" topLeftCell="A1048522" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H1048576" sqref="H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1108,7 +1114,7 @@
     <col min="28" max="28" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -1207,8 +1213,16 @@
       <c r="AI1" s="14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AK1" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="AL1" s="14"/>
+      <c r="AN1" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="AO1" s="14"/>
+    </row>
+    <row r="2" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
@@ -1311,8 +1325,20 @@
       <c r="AI2" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AK2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1415,8 +1441,20 @@
       <c r="AI3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AK3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1519,8 +1557,14 @@
       <c r="AI4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AN4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1623,8 +1667,14 @@
       <c r="AI5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AN5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1727,8 +1777,14 @@
       <c r="AI6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AN6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1808,7 +1864,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1905,8 +1961,14 @@
       <c r="AI8" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AN8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO8" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>87</v>
       </c>
@@ -2004,7 +2066,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2102,7 +2164,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2194,7 +2256,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -2286,7 +2348,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -2384,7 +2446,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -2482,7 +2544,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -2574,7 +2636,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -3442,11 +3504,16 @@
         <v>69</v>
       </c>
     </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="M1:N1"/>
+  <mergeCells count="14">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
@@ -3456,6 +3523,11 @@
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>